<commit_message>
Extratextual analysis by using the transcriptions from WhisperAI
</commit_message>
<xml_diff>
--- a/embrace_books_transcriptions.xlsx
+++ b/embrace_books_transcriptions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jab464/Documents/GitHub/EMBRACE-data-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D39AB5C-DBE4-A846-B63B-65170E55EE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE4608C-7298-5445-99A7-138BA4B913BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="4040" windowWidth="28040" windowHeight="17440" xr2:uid="{98100157-296D-8243-A0EA-AA15D6761731}"/>
+    <workbookView xWindow="15460" yWindow="4000" windowWidth="23300" windowHeight="17240" xr2:uid="{98100157-296D-8243-A0EA-AA15D6761731}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="75">
   <si>
     <t>title</t>
   </si>
@@ -129,12 +129,156 @@
   <si>
     <t>The contest</t>
   </si>
+  <si>
+    <t>La familia López vive en una casa linda. Martin es el papá y es policía. En las mañanas, Martin se va al trabajo. Él toma sus llaves del gancho en la cocina y se monta en su carro. </t>
+  </si>
+  <si>
+    <t>The Lopez Family</t>
+  </si>
+  <si>
+    <t>The Lopez Family Mistery</t>
+  </si>
+  <si>
+    <t>La familia López tiene dos mascotas. Paco, el perro, corre afuera a lamer a Martin para despedirse. Pronto, la familia López tendrá un misterio que resolver. </t>
+  </si>
+  <si>
+    <t>Missing keys</t>
+  </si>
+  <si>
+    <t>Un día, Martin se lavó la cara y desayunó. Caminó hacia el gancho para tomar sus llaves. ¡Pero las llaves no estaban! </t>
+  </si>
+  <si>
+    <t>Martin buscó las llaves por la sala. La familia entera ayudó a Martin, pero no las encontraron. ¿Dónde estaban las llaves? </t>
+  </si>
+  <si>
+    <t>Paco olio algo. Quizás eran las llaves. ¡Entonces vio las llaves en el árbol! Ladro y ladro, y de repente, las llaves cayeron al suelo. </t>
+  </si>
+  <si>
+    <t>Is Paco a thief?</t>
+  </si>
+  <si>
+    <t>More is missing!</t>
+  </si>
+  <si>
+    <t>Al próximo día, Rosa, la mamá, fue a la cocina para hacer panqueques. Ella caminó al fregadero para usar su cuchara de plata y revolver la mezcla. ¡Pero la cuchara no estaba! </t>
+  </si>
+  <si>
+    <t>Martin escucho los ladridos y salió. Martin encontró las llaves cerca de Paco. Martin dijo “¡Paco, eres un mal perro por haberte robado mis llaves! Te tendrás que quedar afuera todo el día. Paco estaba muy triste. </t>
+  </si>
+  <si>
+    <t>Paco corrió hacia el árbol. ¡Ladró y ladró, y la cuchara de plata cayó al suelo! Paco estaba tan contento; ¡resolvió el misterio! Pero la mamá dijo, “Paco, eres un mal perro por robarte mi cuchara de plata. Te tendrás que quedar afuera todo el día” </t>
+  </si>
+  <si>
+    <t>The baby's rattle is gone, too!</t>
+  </si>
+  <si>
+    <t>Mas tarde ese día, la bebé quería jugar con su sonaja. Pero la sonaja estaba desaparecida también. La bebé empezó a llorar. Lola, la conejita, brinco a los brazos de la bebé para hacerla sentir mejor.  </t>
+  </si>
+  <si>
+    <t>Paco escucho la bebé llorar también. ¡Miro hacia el árbol y ahí vio la sonaja! Paco ladro y ladro, y la sonaja cayó al suelo. </t>
+  </si>
+  <si>
+    <t>The mistery is solved</t>
+  </si>
+  <si>
+    <t>Martin guio a su casa y puso sus llaves en el gancho. Martin salió para unirse a su familia cerca del árbol. Entonces, justo ahí vio un pájaro volar del árbol y entrar a la cocina. El pájaro tomo las llaves y volvió hacia su nido. </t>
+  </si>
+  <si>
+    <t>Paco ladró y ladró, y el pájaro soltó las llaves al suelo. ¡Ahora todos entendieron que el pájaro era el ladrón! El misterio finalmente se resolvió. ¡Paco era un héroe! Esa noche, Paco comió un bistec como recompensa. </t>
+  </si>
+  <si>
+    <t>A celebration to remember</t>
+  </si>
+  <si>
+    <t>Key ingredients</t>
+  </si>
+  <si>
+    <t>La familia Romero estaban preparandose para la gran celebración que iban a tener esa noche. ¡Olivia, la hermana de Sofía, se iba a casar! Sofía estaba en la cocina ayudando a su mamá preparar el mole. </t>
+  </si>
+  <si>
+    <t>Sofía agarró el tazón con chiles rojos y se lo dió a su madre para que los moliera. "¡Caramba, Sofía!" dijo su mamá. "¡Olvidamos algunos ingredientes importantes!" </t>
+  </si>
+  <si>
+    <t>Sofía corrió por una libreta y un lápiz, y se los trajo a su mamá."¡Yo voy al mercado y te los traigo!" dijo ella con entusiasmo. </t>
+  </si>
+  <si>
+    <t>Sofía caminó hasta el corral para agarrar a su caballo pinto para el viaje al mercado.  El nombre de su caballo era Mancha, y fue un regalo de su abuelo. </t>
+  </si>
+  <si>
+    <t>Mancha the horse</t>
+  </si>
+  <si>
+    <t>Ella puso la silla de montar en el caballo y ató las correas firmemente como su abuelo le había enseñado. </t>
+  </si>
+  <si>
+    <t>Antes de seguir adelante, Sofía tomó la lista de compras de su bolsa, y la leyó por si se le perdía. Necesitaba comprar tomatillos, leche y espinacas. </t>
+  </si>
+  <si>
+    <t>A friend in need</t>
+  </si>
+  <si>
+    <t>Sofía montó por el camino hacia el mercado. Pero pronto se detuvo ya que había una manada de ganado bloqueando su camino. Su amigo, Emilio, estaba tratando de mover los animales. </t>
+  </si>
+  <si>
+    <t>"¡Sofía! ¡Hola! ¿Puedes ayudarme a meter mi ganado en el corral?" exclamó él. "¡Claro, Emilio!" respondió ella. Sofía ayudó a su amigo cabalgando su caballo detrás y adelante de la manada. </t>
+  </si>
+  <si>
+    <t>"¡Gracias, Sofía!" dijo Emilio con una sonrisa en su rostro.  "Sin tu ayuda, yo seguiría persiguiendo vacas." Luego él se bajó de su caballo y cerró la puerta del corral con su ganado adentro. </t>
+  </si>
+  <si>
+    <t>Shopping at the market</t>
+  </si>
+  <si>
+    <t>Después de ayudarle a su amigo con su ganado, Sofía cabalgó al mercado. </t>
+  </si>
+  <si>
+    <t>Cuando Sofía llegó, saltó de su caballo y lo ató a un poste en frente del mercado. Sofía llevó su bolsa a la sección de frutas y verduras y puso muchos tomatillos en ella.  </t>
+  </si>
+  <si>
+    <t>Ella también puso un manojo de espinaca en la bolsa. Finalmente, Sofía pasó a la sección de productos lácteos y tomó un cartón de leche fresca. </t>
+  </si>
+  <si>
+    <t>Sofía se acercó a la señora Peña y pagó sus compras; el total fueron 30 pesos. Ahora estaba lista para irse a casa. </t>
+  </si>
+  <si>
+    <t>A gift for the bride</t>
+  </si>
+  <si>
+    <t>Sofía subió a su caballo y regresó por el camino para su casa. Ella estaba feliz de que su salida fuera tan exitosa, pero tenía la sensación de que estaba olvidando algo. </t>
+  </si>
+  <si>
+    <t>Sofia las llevó al frente para pagar. "¡A tu hermana le van a gustar mucho estas flores, Sofía!" dijo la señora Peña. </t>
+  </si>
+  <si>
+    <t>Sofía cabalgó el resto del camino a casa y llevó su caballo al corral. </t>
+  </si>
+  <si>
+    <t>Homecoming</t>
+  </si>
+  <si>
+    <t>Sofía regresó a casa, esta vez segura de que había comprado todo lo que necesitaba. </t>
+  </si>
+  <si>
+    <t>Sofía vació la bolsa en el mostrador y dijo, "Aquí está todo lo que pediste, mamá. ¡Incluso tuve suficiente dinero para comprarle estas rosas a Olivia!" </t>
+  </si>
+  <si>
+    <t>La madre de Sofía se acercó al mostrador y examinó las compras.  La mamá dijo: "¡Has hecho un gran trabajo escogiendo las frutas y verduras más fresca, Sofía! Ahora podemos tener una fiesta." Sofía decidió hacer una última cosa antes de unirse a la fiesta. </t>
+  </si>
+  <si>
+    <t>Sofia puso las rosas en el florero para que Olivia las pudiera disfrutar por más tiempo. ¡Sofía felizmente corrió desde la cocina para unirse a lo que iba a ser una celebración inolvidable! </t>
+  </si>
+  <si>
+    <t>Y luego recordó que ella quería usar el resto del dinero para comprar un regalo de bodas para Olivia, su hermana mayor. Se dio la vuelta y cabalgó lo más rápido que pudo para regresar al mercado. </t>
+  </si>
+  <si>
+    <t>Sofía se acercó a las rosas y escogió una docena de rosas rosadas y una docena de rosas blancas. Las rosas rosadas mostraban el amor de Sofía por Olivia, y las rosas blancas mostraban el amor entre la novia y el novio. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -144,6 +288,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -170,9 +321,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA44D987-DFD5-9F41-8229-9BA2D2E72189}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,135 +653,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
@@ -637,16 +789,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
@@ -654,16 +806,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
         <v>5</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
@@ -671,16 +823,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
         <v>5</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
@@ -688,16 +840,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
         <v>6</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
@@ -705,16 +857,16 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
         <v>6</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
@@ -722,16 +874,16 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
         <v>7</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
@@ -739,20 +891,598 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
         <v>7</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="1">
+        <v>6</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>